<commit_message>
modified:   WebRoot/page/auditmetro.xlsx 	modified:   src/com/cn/common/factory/PoiBidAccountReport.java 	modified:   src/com/cn/common/factory/PoiBidDataReport.java 	modified:   src/com/cn/common/factory/PoiBidEngineerReport.java 	new file:   src/com/cn/common/factory/PoiBidNeiyeReport.java 	modified:   src/com/cn/common/factory/PoiExpertPayReport.java 	modified:   src/com/cn/tbps/dto/BidDto.java 	modified:   src/com/cn/tbps/dto/BidRptDto.java
</commit_message>
<xml_diff>
--- a/WebRoot/page/auditmetro.xlsx
+++ b/WebRoot/page/auditmetro.xlsx
@@ -113,9 +113,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,7 +150,7 @@
     <font>
       <sz val="12"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -164,12 +164,6 @@
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -343,11 +337,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +433,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,9 +493,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -462,54 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -950,8 +941,8 @@
   </sheetPr>
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8:T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -960,29 +951,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="1"/>
@@ -1008,13 +999,13 @@
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1035,164 +1026,164 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="39" t="s">
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="40" t="s">
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
     </row>
     <row r="5" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="41" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="39" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="44" t="s">
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
     </row>
     <row r="6" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="44" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="45" t="s">
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
     </row>
     <row r="7" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="40" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
       <c r="K7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="40" t="s">
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
       <c r="U7" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
       <c r="N8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="39" t="s">
+      <c r="O8" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="47" t="s">
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
       <c r="U8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1244,33 +1235,33 @@
       <c r="U10" s="9"/>
     </row>
     <row r="11" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="48" t="s">
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="50"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="33"/>
     </row>
     <row r="12" spans="1:21" ht="21.95" customHeight="1">
       <c r="A12" s="10"/>
@@ -1319,62 +1310,62 @@
       <c r="U13" s="29"/>
     </row>
     <row r="14" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="48" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="48" t="s">
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="49"/>
-      <c r="U14" s="50"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="33"/>
     </row>
     <row r="15" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="48" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="48" t="s">
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="50"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="33"/>
     </row>
     <row r="16" spans="1:21" ht="21.95" customHeight="1">
       <c r="A16" s="14"/>
@@ -1427,8 +1418,8 @@
         <v>28</v>
       </c>
       <c r="B18" s="22"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1449,6 +1440,31 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:T8"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="H15:N15"/>
     <mergeCell ref="O15:U15"/>
@@ -1459,33 +1475,8 @@
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="H14:N14"/>
     <mergeCell ref="O14:U14"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:U5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:U4"/>
   </mergeCells>
-  <phoneticPr fontId="10"/>
+  <phoneticPr fontId="9"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70763888888888904" right="0.70763888888888904" top="0.74791666666666701" bottom="0.74791666666666701" header="0.31388888888888899" footer="0.31388888888888899"/>
   <pageSetup paperSize="9" scale="96" orientation="landscape"/>

</xml_diff>